<commit_message>
Cleaned up for review
</commit_message>
<xml_diff>
--- a/SummarizeResultDrill.xlsx
+++ b/SummarizeResultDrill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{AD247665-3D5E-4780-89C3-359FA6FD3D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{6530D909-15C8-45D9-B0DA-B362228327B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -890,6 +890,35 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="882" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{C2C58A28-D8AB-4B7F-B821-1954FE041EAA}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{0C1EBD7A-6299-43A9-9268-753300CC1BC7}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1">
@@ -897,8 +926,8 @@
   </sheetPr>
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="H6" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -972,7 +1001,24 @@
         <v>4</v>
       </c>
       <c r="N6" s="2" t="str" cm="1">
-        <f t="array" ref="N6:S11">_xlfn.MAKEARRAY(6,6,_xlfn.LAMBDA(_xlpm.r,_xlpm.c,_xlfn.IFS(_xlpm.r*_xlpm.c=1,"",_xlpm.r=1,_xlpm.c-1,_xlpm.c=1,_xlpm.r-1,TRUE,_xlfn.ARRAYTOTEXT(_xlfn._xlws.FILTER(A2:A10,(B2:B10=_xlpm.r-1)*(C2:C10=_xlpm.c-1),"")))))</f>
+        <f t="array" ref="N6:S11">_xlfn.MAKEARRAY(
+    6,
+    6,
+    _xlfn.LAMBDA(_xlpm.r,_xlpm.c,
+        _xlfn.IFS(
+            _xlpm.r * _xlpm.c = 1,
+            "",
+            _xlpm.r = 1,
+            _xlpm.c - 1,
+            _xlpm.c = 1,
+            _xlpm.r - 1,
+            TRUE,
+            _xlfn.ARRAYTOTEXT(
+                _xlfn._xlws.FILTER(A2:A10, (B2:B10 = _xlpm.r - 1) * (C2:C10 = _xlpm.c - 1), "")
+            )
+        )
+    )
+)</f>
         <v/>
       </c>
       <c r="O6" s="2">
@@ -1131,4 +1177,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C1EBD7A-6299-43A9-9268-753300CC1BC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>